<commit_message>
Actualizacion de flujo Con Seleniun
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/DATA_DELIVERY_MOVISTAR.xlsx
+++ b/src/main/resources/excel/DATA_DELIVERY_MOVISTAR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FramerworkTsoft\Movistar\web-automation-movistar\src\main\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B75F3464-80A9-4734-BB22-42A3FF8F8745}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF29D40F-C670-4440-BDB0-D1BF9FA5491E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{889843C2-4537-4BE6-8724-CE3764E265B9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{889843C2-4537-4BE6-8724-CE3764E265B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Direccion" sheetId="1" r:id="rId1"/>
@@ -4035,9 +4035,6 @@
     <t>Titular</t>
   </si>
   <si>
-    <t>Intrucciones</t>
-  </si>
-  <si>
     <t>HorarioEntrega</t>
   </si>
   <si>
@@ -4054,6 +4051,9 @@
   </si>
   <si>
     <t>Parque Zonal 3</t>
+  </si>
+  <si>
+    <t>Instrucciones</t>
   </si>
 </sst>
 </file>
@@ -4495,7 +4495,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CF93585-9459-4212-A3A6-B60B4F01B565}">
   <dimension ref="A1:F1370"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
@@ -4543,7 +4543,7 @@
         <v>1254</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -19662,7 +19662,7 @@
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="F2" s="3">
         <v>7</v>
@@ -19677,13 +19677,13 @@
         <v>1267</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>1301</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -19769,10 +19769,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2C91567-216F-4355-8FE2-AB19DE846802}">
-  <dimension ref="A7:E15"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19783,30 +19783,32 @@
     <col min="5" max="5" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
-        <v>1336</v>
-      </c>
-      <c r="B7" s="6" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>1335</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>1332</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C1" s="6" t="s">
         <v>1333</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D1" s="6" t="s">
+        <v>1340</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>1334</v>
       </c>
-      <c r="E7" s="6" t="s">
-        <v>1335</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B8" s="3" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
         <v>1321</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3" t="s">
+      <c r="C2" s="3">
+        <v>979586095</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3" t="s">
         <v>1326</v>
       </c>
     </row>
@@ -19861,13 +19863,13 @@
           <x14:formula1>
             <xm:f>DATOS!$I$4:$I$8</xm:f>
           </x14:formula1>
-          <xm:sqref>B8</xm:sqref>
+          <xm:sqref>B2</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ERROR DE DATA" error="POR FAVOR_x000a_Seleccione un horario de la lista" xr:uid="{00AD6229-B302-44EB-BE12-24EB7AC37442}">
           <x14:formula1>
             <xm:f>DATOS!$K$4:$K$5</xm:f>
           </x14:formula1>
-          <xm:sqref>E8</xm:sqref>
+          <xm:sqref>E2</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Se agrego la carga de audio
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/DATA_DELIVERY_MOVISTAR.xlsx
+++ b/src/main/resources/excel/DATA_DELIVERY_MOVISTAR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FramerworkTsoft\Movistar\web-automation-movistar\src\main\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF29D40F-C670-4440-BDB0-D1BF9FA5491E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2890226-E16C-4E9C-A7B6-7B3AE039EF44}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{889843C2-4537-4BE6-8724-CE3764E265B9}"/>
   </bookViews>
@@ -19772,7 +19772,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>